<commit_message>
admin and gibson assembly updates
added chemical managment, edited purchasing

edited Gibson assembly to emphasize that you don't need to clean PCR products for Gibson
</commit_message>
<xml_diff>
--- a/workbooks/assembly_workbook.xlsx
+++ b/workbooks/assembly_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiffl\Documents\GitHub\protocols\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E638388C-E5A4-4B81-B943-E0331652C148}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3506A0D5-F717-4594-BD44-04E38E76001E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12924" windowHeight="8520" xr2:uid="{DCF1C1EE-0D39-48BA-A8AB-FBDE3A309C29}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DCF1C1EE-0D39-48BA-A8AB-FBDE3A309C29}"/>
   </bookViews>
   <sheets>
     <sheet name="10 ul" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'10 ul'!$A$8:$N$64</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>NEB recommends a total of 0.015–0.1 pmols of DNA fragments when 1 or 2 fragments are being assembled into a vector, and 0.1–0.25 pmols of DNA fragments when 4–6 fragments are being assembled. </t>
-  </si>
-  <si>
-    <t>Purification of PCR products is generally not necessary. You can use unpurified PCR products directly, as long as the total volume of PCR products in the Assembly reaction is 20% or less. If greater amounts of PCR products are used, a column cleanup kit is sufficient. It is advantageous to gel-purify the target DNA fragment if the PCR product is contaminated by either non-specific amplification products, primer-dimers or large quantities of unused PCR primers.</t>
   </si>
   <si>
     <t>(AKA pUC18t-miniTn7-Gm)</t>
@@ -172,6 +169,27 @@
       <t>,</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF3A3A3A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Purification of PCR products is generally not necessary.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3A3A3A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> You can use unpurified PCR products directly, as long as the total volume of PCR products in the Assembly reaction is 20% or less. If greater amounts of PCR products are used, a column cleanup kit is sufficient. It is advantageous to gel-purify the target DNA fragment if the PCR product is contaminated by either non-specific amplification products, primer-dimers or large quantities of unused PCR primers.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -181,7 +199,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +327,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -684,10 +709,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC310"/>
+  <dimension ref="A1:N310"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,22 +739,22 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -744,7 +769,7 @@
     </row>
     <row r="8" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -768,7 +793,7 @@
     </row>
     <row r="12" spans="1:14" s="22" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="22">
         <v>4569</v>
@@ -777,7 +802,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="22" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -972,7 +997,7 @@
         <v>5</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -1188,7 +1213,7 @@
         <v>5</v>
       </c>
       <c r="L32" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -1449,7 +1474,7 @@
         <v>5</v>
       </c>
       <c r="L44" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.3"/>

</xml_diff>